<commit_message>
Work through section 4 - pandas overview
</commit_message>
<xml_diff>
--- a/Udemy-Time-Series-Analysis/02-Pandas/Excel_Sample.xlsx
+++ b/Udemy-Time-Series-Analysis/02-Pandas/Excel_Sample.xlsx
@@ -12,23 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,21 +366,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -414,7 +405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -431,7 +422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -448,7 +439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>

</xml_diff>